<commit_message>
Nuevo cambio a flujo de caja
</commit_message>
<xml_diff>
--- a/FLUJO.xlsx
+++ b/FLUJO.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20225"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14200" tabRatio="884" activeTab="9"/>
+    <workbookView xWindow="6420" yWindow="0" windowWidth="25600" windowHeight="20480" tabRatio="884" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="FLUJO CAJA 1" sheetId="8" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="131">
   <si>
     <t>INVERSIÓN</t>
   </si>
@@ -418,6 +418,9 @@
   </si>
   <si>
     <t>Presupuesto adhoc de marketing</t>
+  </si>
+  <si>
+    <t>Tasa Crecimiento CF</t>
   </si>
 </sst>
 </file>
@@ -532,7 +535,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="36">
+  <borders count="37">
     <border>
       <left/>
       <right/>
@@ -954,6 +957,17 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="double">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom style="double">
         <color auto="1"/>
       </bottom>
@@ -979,7 +993,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="192">
+  <cellXfs count="196">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1267,18 +1281,54 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="3" fontId="2" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="4" borderId="33" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="4" borderId="34" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="4" borderId="35" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="4" borderId="33" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="4" borderId="35" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1288,41 +1338,17 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="4" borderId="34" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1336,49 +1362,43 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="4" fillId="4" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="17">
-    <cellStyle name="Hipervínculo" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Moneda" xfId="2" builtinId="4"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Porcentual" xfId="1" builtinId="5"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Percentuale" xfId="1" builtinId="5"/>
+    <cellStyle name="Valuta" xfId="2" builtinId="4"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1750,10 +1770,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:L27"/>
+  <dimension ref="B4:L31"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView topLeftCell="D2" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1761,7 +1781,7 @@
     <col min="1" max="1" width="6.33203125" customWidth="1"/>
     <col min="2" max="2" width="4.6640625" customWidth="1"/>
     <col min="3" max="3" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" customWidth="1"/>
     <col min="5" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13" bestFit="1" customWidth="1"/>
@@ -1909,7 +1929,7 @@
       </c>
       <c r="L8">
         <f>D22/6</f>
-        <v>20961588.977240089</v>
+        <v>11534314.579725521</v>
       </c>
     </row>
     <row r="9" spans="2:12">
@@ -1958,24 +1978,24 @@
         <v>-113378600</v>
       </c>
       <c r="F10" s="107">
-        <f>E10*115%</f>
-        <v>-130385389.99999999</v>
+        <f>E10*(1+$D$27)</f>
+        <v>-136054320</v>
       </c>
       <c r="G10" s="107">
-        <f t="shared" ref="G10:J10" si="0">F10*115%</f>
-        <v>-149943198.49999997</v>
+        <f t="shared" ref="G10:J10" si="0">F10*(1+$D$27)</f>
+        <v>-163265184</v>
       </c>
       <c r="H10" s="107">
         <f t="shared" si="0"/>
-        <v>-172434678.27499995</v>
+        <v>-195918220.79999998</v>
       </c>
       <c r="I10" s="107">
         <f t="shared" si="0"/>
-        <v>-198299880.01624992</v>
+        <v>-235101864.95999998</v>
       </c>
       <c r="J10" s="107">
         <f t="shared" si="0"/>
-        <v>-228044862.0186874</v>
+        <v>-282122237.95199996</v>
       </c>
     </row>
     <row r="11" spans="2:12">
@@ -2025,23 +2045,23 @@
       </c>
       <c r="F12" s="109">
         <f t="shared" si="1"/>
-        <v>16246443.333333349</v>
+        <v>10577513.333333334</v>
       </c>
       <c r="G12" s="109">
         <f t="shared" si="1"/>
-        <v>38559784.833333366</v>
+        <v>25237799.333333332</v>
       </c>
       <c r="H12" s="109">
         <f t="shared" si="1"/>
-        <v>69670861.596794948</v>
+        <v>46187319.07179492</v>
       </c>
       <c r="I12" s="109">
         <f t="shared" si="1"/>
-        <v>112467520.63365148</v>
+        <v>75665535.689901426</v>
       </c>
       <c r="J12" s="109">
         <f t="shared" si="1"/>
-        <v>170725772.75426811</v>
+        <v>116648396.82095553</v>
       </c>
     </row>
     <row r="13" spans="2:12">
@@ -2091,23 +2111,23 @@
       </c>
       <c r="F14" s="109">
         <f t="shared" si="2"/>
-        <v>13407118.467768604</v>
+        <v>7738188.467768589</v>
       </c>
       <c r="G14" s="109">
         <f t="shared" si="2"/>
-        <v>35720459.967768617</v>
+        <v>22398474.467768587</v>
       </c>
       <c r="H14" s="109">
         <f t="shared" si="2"/>
-        <v>66831536.731230199</v>
+        <v>43347994.206230171</v>
       </c>
       <c r="I14" s="109">
         <f t="shared" si="2"/>
-        <v>109628195.76808673</v>
+        <v>72826210.824336678</v>
       </c>
       <c r="J14" s="109">
         <f t="shared" si="2"/>
-        <v>167886447.88870338</v>
+        <v>113809071.95539078</v>
       </c>
     </row>
     <row r="15" spans="2:12">
@@ -2124,23 +2144,23 @@
       </c>
       <c r="F15" s="107">
         <f t="shared" si="3"/>
-        <v>-2279210.1395206628</v>
+        <v>-1315492.0395206602</v>
       </c>
       <c r="G15" s="107">
         <f t="shared" si="3"/>
-        <v>-6072478.1945206653</v>
+        <v>-3807740.6595206601</v>
       </c>
       <c r="H15" s="107">
         <f t="shared" si="3"/>
-        <v>-11361361.244309135</v>
+        <v>-7369159.0150591293</v>
       </c>
       <c r="I15" s="107">
         <f t="shared" si="3"/>
-        <v>-18636793.280574746</v>
+        <v>-12380455.840137236</v>
       </c>
       <c r="J15" s="107">
         <f t="shared" si="3"/>
-        <v>-28540696.141079575</v>
+        <v>-19347542.232416432</v>
       </c>
     </row>
     <row r="16" spans="2:12">
@@ -2232,7 +2252,7 @@
       <c r="C19" s="83" t="s">
         <v>81</v>
       </c>
-      <c r="D19" s="110">
+      <c r="D19" s="195">
         <f>'G. FINANCIERO'!C5</f>
         <v>12366000</v>
       </c>
@@ -2260,23 +2280,23 @@
       </c>
       <c r="F20" s="131">
         <f t="shared" si="5"/>
-        <v>9593574.9949146081</v>
+        <v>4888363.0949145956</v>
       </c>
       <c r="G20" s="131">
         <f t="shared" si="5"/>
-        <v>28113648.439914618</v>
+        <v>17056400.474914595</v>
       </c>
       <c r="H20" s="131">
         <f t="shared" si="5"/>
-        <v>53935842.153587729</v>
+        <v>34444501.857837707</v>
       </c>
       <c r="I20" s="131">
         <f t="shared" si="5"/>
-        <v>89457069.154178664</v>
+        <v>58911421.650866106</v>
       </c>
       <c r="J20" s="131">
         <f t="shared" si="5"/>
-        <v>137811418.41429046</v>
+        <v>92927196.389641017</v>
       </c>
     </row>
     <row r="21" spans="2:10" ht="13" thickBot="1">
@@ -2289,23 +2309,23 @@
       </c>
       <c r="F21" s="137">
         <f>F20+E21</f>
-        <v>-6797849.8706501368</v>
+        <v>-11503061.770650148</v>
       </c>
       <c r="G21" s="137">
         <f>G20+F21</f>
-        <v>21315798.569264479</v>
+        <v>5553338.7042644471</v>
       </c>
       <c r="H21" s="137">
         <f>H20+G21</f>
-        <v>75251640.7228522</v>
+        <v>39997840.562102154</v>
       </c>
       <c r="I21" s="137">
         <f>I20+H21</f>
-        <v>164708709.87703085</v>
+        <v>98909262.21296826</v>
       </c>
       <c r="J21" s="137">
         <f>J20+I21</f>
-        <v>302520128.29132128</v>
+        <v>191836458.60260928</v>
       </c>
     </row>
     <row r="22" spans="2:10">
@@ -2315,12 +2335,12 @@
       </c>
       <c r="D22" s="143">
         <f>NPV(D24,E20:J20)+D18</f>
-        <v>125769533.86344054</v>
+        <v>69205887.478353128</v>
       </c>
       <c r="E22" s="137"/>
       <c r="F22" s="139">
         <f>D22/D18</f>
-        <v>-6.1023548696477699</v>
+        <v>-3.3578790625110688</v>
       </c>
       <c r="G22" s="137"/>
       <c r="H22" s="137"/>
@@ -2334,7 +2354,7 @@
       </c>
       <c r="D23" s="144">
         <f>IRR(D20:J20)</f>
-        <v>0.91807730821074163</v>
+        <v>0.68463232915470229</v>
       </c>
       <c r="E23" s="136"/>
       <c r="F23" s="141"/>
@@ -2359,8 +2379,20 @@
       <c r="J24" s="136"/>
     </row>
     <row r="27" spans="2:10">
+      <c r="C27" s="192" t="s">
+        <v>130</v>
+      </c>
+      <c r="D27" s="193">
+        <v>0.2</v>
+      </c>
       <c r="I27" t="s">
         <v>85</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10">
+      <c r="D31" s="194">
+        <f>-D22/D18</f>
+        <v>3.3578790625110688</v>
       </c>
     </row>
   </sheetData>
@@ -2379,7 +2411,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -2425,8 +2457,8 @@
   <sheetPr codeName="Hoja2" enableFormatConditionsCalculation="0"/>
   <dimension ref="B3:D20"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -2673,30 +2705,30 @@
     <row r="4" spans="2:16" ht="13" thickBot="1">
       <c r="B4" s="101"/>
       <c r="C4" s="101"/>
-      <c r="D4" s="175" t="s">
+      <c r="D4" s="173" t="s">
         <v>93</v>
       </c>
-      <c r="E4" s="177"/>
-      <c r="F4" s="175" t="s">
+      <c r="E4" s="175"/>
+      <c r="F4" s="173" t="s">
         <v>96</v>
       </c>
-      <c r="G4" s="176"/>
-      <c r="H4" s="177" t="s">
+      <c r="G4" s="174"/>
+      <c r="H4" s="175" t="s">
         <v>97</v>
       </c>
-      <c r="I4" s="177"/>
-      <c r="J4" s="175" t="s">
+      <c r="I4" s="175"/>
+      <c r="J4" s="173" t="s">
         <v>98</v>
       </c>
-      <c r="K4" s="176"/>
-      <c r="L4" s="177" t="s">
+      <c r="K4" s="174"/>
+      <c r="L4" s="175" t="s">
         <v>99</v>
       </c>
-      <c r="M4" s="177"/>
-      <c r="N4" s="175" t="s">
+      <c r="M4" s="175"/>
+      <c r="N4" s="173" t="s">
         <v>100</v>
       </c>
-      <c r="O4" s="176"/>
+      <c r="O4" s="174"/>
       <c r="P4" s="101"/>
     </row>
     <row r="5" spans="2:16" ht="13" thickBot="1">
@@ -2742,7 +2774,7 @@
     </row>
     <row r="6" spans="2:16" ht="13" thickBot="1">
       <c r="B6" s="101"/>
-      <c r="C6" s="165" t="s">
+      <c r="C6" s="177" t="s">
         <v>89</v>
       </c>
       <c r="D6" s="148">
@@ -2791,42 +2823,42 @@
     </row>
     <row r="7" spans="2:16" ht="13" thickBot="1">
       <c r="B7" s="101"/>
-      <c r="C7" s="166"/>
-      <c r="D7" s="168">
+      <c r="C7" s="178"/>
+      <c r="D7" s="167">
         <f>D6*E6</f>
         <v>43200000</v>
       </c>
-      <c r="E7" s="169"/>
-      <c r="F7" s="168">
+      <c r="E7" s="172"/>
+      <c r="F7" s="167">
         <f>F6*G6</f>
         <v>56160000</v>
       </c>
-      <c r="G7" s="170"/>
-      <c r="H7" s="169">
+      <c r="G7" s="168"/>
+      <c r="H7" s="172">
         <f>H6*I6</f>
         <v>69120000</v>
       </c>
-      <c r="I7" s="169"/>
-      <c r="J7" s="168">
+      <c r="I7" s="172"/>
+      <c r="J7" s="167">
         <f>J6*K6</f>
         <v>85070769.230769232</v>
       </c>
-      <c r="K7" s="170"/>
-      <c r="L7" s="169">
+      <c r="K7" s="168"/>
+      <c r="L7" s="172">
         <f>L6*M6</f>
         <v>104702485.2071006</v>
       </c>
-      <c r="M7" s="169"/>
-      <c r="N7" s="168">
+      <c r="M7" s="172"/>
+      <c r="N7" s="167">
         <f>N6*O6</f>
         <v>128864597.17796996</v>
       </c>
-      <c r="O7" s="170"/>
+      <c r="O7" s="168"/>
       <c r="P7" s="101"/>
     </row>
     <row r="8" spans="2:16" ht="13" thickBot="1">
       <c r="B8" s="101"/>
-      <c r="C8" s="165" t="s">
+      <c r="C8" s="177" t="s">
         <v>114</v>
       </c>
       <c r="D8" s="111">
@@ -2875,42 +2907,42 @@
     </row>
     <row r="9" spans="2:16" ht="13" thickBot="1">
       <c r="B9" s="101"/>
-      <c r="C9" s="167"/>
-      <c r="D9" s="171">
+      <c r="C9" s="179"/>
+      <c r="D9" s="170">
         <f>D8*E8</f>
         <v>6300000</v>
       </c>
-      <c r="E9" s="162"/>
-      <c r="F9" s="171">
+      <c r="E9" s="169"/>
+      <c r="F9" s="170">
         <f>F8*G8</f>
         <v>3290000</v>
       </c>
-      <c r="G9" s="178"/>
-      <c r="H9" s="162">
+      <c r="G9" s="171"/>
+      <c r="H9" s="169">
         <f>H8*I8</f>
         <v>4277000</v>
       </c>
-      <c r="I9" s="162"/>
-      <c r="J9" s="171">
+      <c r="I9" s="169"/>
+      <c r="J9" s="170">
         <f>J8*K8</f>
         <v>5560100.0000000019</v>
       </c>
-      <c r="K9" s="178"/>
-      <c r="L9" s="162">
+      <c r="K9" s="171"/>
+      <c r="L9" s="169">
         <f>L8*M8</f>
         <v>7228130</v>
       </c>
-      <c r="M9" s="162"/>
-      <c r="N9" s="171">
+      <c r="M9" s="169"/>
+      <c r="N9" s="170">
         <f>N8*O8</f>
         <v>9396569</v>
       </c>
-      <c r="O9" s="178"/>
+      <c r="O9" s="171"/>
       <c r="P9" s="101"/>
     </row>
     <row r="10" spans="2:16" ht="13" thickBot="1">
       <c r="B10" s="101"/>
-      <c r="C10" s="166" t="s">
+      <c r="C10" s="178" t="s">
         <v>90</v>
       </c>
       <c r="D10" s="111">
@@ -2964,42 +2996,42 @@
     </row>
     <row r="11" spans="2:16" ht="13" thickBot="1">
       <c r="B11" s="101"/>
-      <c r="C11" s="166"/>
-      <c r="D11" s="168">
+      <c r="C11" s="178"/>
+      <c r="D11" s="167">
         <f>D10*E10</f>
         <v>60000000</v>
       </c>
-      <c r="E11" s="169"/>
-      <c r="F11" s="168">
+      <c r="E11" s="172"/>
+      <c r="F11" s="167">
         <f>F10*G10</f>
         <v>78000000</v>
       </c>
-      <c r="G11" s="170"/>
-      <c r="H11" s="169">
+      <c r="G11" s="168"/>
+      <c r="H11" s="172">
         <f>H10*I10</f>
         <v>101400000</v>
       </c>
-      <c r="I11" s="169"/>
-      <c r="J11" s="168">
+      <c r="I11" s="172"/>
+      <c r="J11" s="167">
         <f>J10*K10</f>
         <v>131820000.00000001</v>
       </c>
-      <c r="K11" s="170"/>
-      <c r="L11" s="169">
+      <c r="K11" s="168"/>
+      <c r="L11" s="172">
         <f>L10*M10</f>
         <v>171366000</v>
       </c>
-      <c r="M11" s="169"/>
-      <c r="N11" s="168">
+      <c r="M11" s="172"/>
+      <c r="N11" s="167">
         <f>N10*O10</f>
         <v>222775800</v>
       </c>
-      <c r="O11" s="170"/>
+      <c r="O11" s="168"/>
       <c r="P11" s="101"/>
     </row>
     <row r="12" spans="2:16" ht="13" thickBot="1">
       <c r="B12" s="101"/>
-      <c r="C12" s="165" t="s">
+      <c r="C12" s="177" t="s">
         <v>122</v>
       </c>
       <c r="D12" s="111"/>
@@ -3048,42 +3080,42 @@
     </row>
     <row r="13" spans="2:16" ht="13" thickBot="1">
       <c r="B13" s="101"/>
-      <c r="C13" s="167"/>
-      <c r="D13" s="171">
+      <c r="C13" s="179"/>
+      <c r="D13" s="170">
         <f>D12*E12</f>
         <v>0</v>
       </c>
-      <c r="E13" s="162"/>
-      <c r="F13" s="171">
+      <c r="E13" s="169"/>
+      <c r="F13" s="170">
         <f>F12*G12</f>
         <v>10920000</v>
       </c>
-      <c r="G13" s="178"/>
-      <c r="H13" s="162">
+      <c r="G13" s="171"/>
+      <c r="H13" s="169">
         <f>H12*I12</f>
         <v>14196000</v>
       </c>
-      <c r="I13" s="162"/>
-      <c r="J13" s="171">
+      <c r="I13" s="169"/>
+      <c r="J13" s="170">
         <f>J12*K12</f>
         <v>18454800</v>
       </c>
-      <c r="K13" s="178"/>
-      <c r="L13" s="162">
+      <c r="K13" s="171"/>
+      <c r="L13" s="169">
         <f>L12*M12</f>
         <v>23991240</v>
       </c>
-      <c r="M13" s="162"/>
-      <c r="N13" s="171">
+      <c r="M13" s="169"/>
+      <c r="N13" s="170">
         <f>N12*O12</f>
         <v>31188612</v>
       </c>
-      <c r="O13" s="178"/>
+      <c r="O13" s="171"/>
       <c r="P13" s="101"/>
     </row>
     <row r="14" spans="2:16" ht="13" thickBot="1">
       <c r="B14" s="101"/>
-      <c r="C14" s="166" t="s">
+      <c r="C14" s="178" t="s">
         <v>94</v>
       </c>
       <c r="D14" s="111"/>
@@ -3127,42 +3159,42 @@
     </row>
     <row r="15" spans="2:16" ht="13" thickBot="1">
       <c r="B15" s="101"/>
-      <c r="C15" s="166"/>
-      <c r="D15" s="168">
+      <c r="C15" s="178"/>
+      <c r="D15" s="167">
         <f>D14*E14</f>
         <v>0</v>
       </c>
-      <c r="E15" s="169"/>
-      <c r="F15" s="168">
+      <c r="E15" s="172"/>
+      <c r="F15" s="167">
         <f>F14*G14</f>
         <v>1950000</v>
       </c>
-      <c r="G15" s="170"/>
-      <c r="H15" s="169">
+      <c r="G15" s="168"/>
+      <c r="H15" s="172">
         <f>H14*I14</f>
         <v>2535000</v>
       </c>
-      <c r="I15" s="169"/>
-      <c r="J15" s="168">
+      <c r="I15" s="172"/>
+      <c r="J15" s="167">
         <f>J14*K14</f>
         <v>3295500</v>
       </c>
-      <c r="K15" s="170"/>
-      <c r="L15" s="169">
+      <c r="K15" s="168"/>
+      <c r="L15" s="172">
         <f>L14*M14</f>
         <v>4284150</v>
       </c>
-      <c r="M15" s="169"/>
-      <c r="N15" s="168">
+      <c r="M15" s="172"/>
+      <c r="N15" s="167">
         <f>N14*O14</f>
         <v>5569395</v>
       </c>
-      <c r="O15" s="170"/>
+      <c r="O15" s="168"/>
       <c r="P15" s="101"/>
     </row>
     <row r="16" spans="2:16" ht="13" thickBot="1">
       <c r="B16" s="101"/>
-      <c r="C16" s="165" t="s">
+      <c r="C16" s="177" t="s">
         <v>95</v>
       </c>
       <c r="D16" s="111"/>
@@ -3206,37 +3238,37 @@
     </row>
     <row r="17" spans="2:16" ht="13" thickBot="1">
       <c r="B17" s="101"/>
-      <c r="C17" s="167"/>
+      <c r="C17" s="179"/>
       <c r="D17" s="163">
         <f>D16*E16</f>
         <v>0</v>
       </c>
-      <c r="E17" s="164"/>
+      <c r="E17" s="166"/>
       <c r="F17" s="163">
         <f>F16*G16</f>
         <v>6500000</v>
       </c>
-      <c r="G17" s="179"/>
-      <c r="H17" s="164">
+      <c r="G17" s="164"/>
+      <c r="H17" s="166">
         <f>H16*I16</f>
         <v>8450000</v>
       </c>
-      <c r="I17" s="164"/>
+      <c r="I17" s="166"/>
       <c r="J17" s="163">
         <f>J16*K16</f>
         <v>10985000</v>
       </c>
-      <c r="K17" s="179"/>
-      <c r="L17" s="164">
+      <c r="K17" s="164"/>
+      <c r="L17" s="166">
         <f>L16*M16</f>
         <v>14280500</v>
       </c>
-      <c r="M17" s="164"/>
+      <c r="M17" s="166"/>
       <c r="N17" s="163">
         <f>N16*O16</f>
         <v>18564650</v>
       </c>
-      <c r="O17" s="179"/>
+      <c r="O17" s="164"/>
       <c r="P17" s="101"/>
     </row>
     <row r="18" spans="2:16" ht="13" thickBot="1">
@@ -3244,36 +3276,36 @@
       <c r="C18" s="105" t="s">
         <v>101</v>
       </c>
-      <c r="D18" s="172">
+      <c r="D18" s="161">
         <f>D7+D9+D11+D13+D15+D17</f>
         <v>109500000</v>
       </c>
-      <c r="E18" s="173"/>
-      <c r="F18" s="172">
+      <c r="E18" s="165"/>
+      <c r="F18" s="161">
         <f>F7+F9+F11+F13+F15+F17</f>
         <v>156820000</v>
       </c>
-      <c r="G18" s="174"/>
-      <c r="H18" s="173">
+      <c r="G18" s="162"/>
+      <c r="H18" s="165">
         <f>H7+H9+H11+H13+H15+H17</f>
         <v>199978000</v>
       </c>
-      <c r="I18" s="173"/>
-      <c r="J18" s="172">
+      <c r="I18" s="165"/>
+      <c r="J18" s="161">
         <f>J7+J9+J11+J13+J15+J17</f>
         <v>255186169.23076925</v>
       </c>
-      <c r="K18" s="174"/>
-      <c r="L18" s="173">
+      <c r="K18" s="162"/>
+      <c r="L18" s="165">
         <f>L7+L9+L11+L13+L15+L17</f>
         <v>325852505.20710063</v>
       </c>
-      <c r="M18" s="173"/>
-      <c r="N18" s="172">
+      <c r="M18" s="165"/>
+      <c r="N18" s="161">
         <f>N7+N9+N11+N13+N15+N17</f>
         <v>416359623.17796993</v>
       </c>
-      <c r="O18" s="174"/>
+      <c r="O18" s="162"/>
       <c r="P18" s="101"/>
     </row>
     <row r="19" spans="2:16">
@@ -3310,12 +3342,12 @@
       <c r="P20" s="101"/>
     </row>
     <row r="21" spans="2:16">
-      <c r="C21" s="161" t="s">
+      <c r="C21" s="176" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="22" spans="2:16">
-      <c r="C22" s="161"/>
+      <c r="C22" s="176"/>
     </row>
     <row r="23" spans="2:16">
       <c r="C23" s="149">
@@ -3348,45 +3380,6 @@
     </row>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="N18:O18"/>
-    <mergeCell ref="N17:O17"/>
-    <mergeCell ref="L18:M18"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="L17:M17"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="N15:O15"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="N13:O13"/>
-    <mergeCell ref="L15:M15"/>
-    <mergeCell ref="N9:O9"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="L11:M11"/>
-    <mergeCell ref="N11:O11"/>
-    <mergeCell ref="L9:M9"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="J9:K9"/>
-    <mergeCell ref="N4:O4"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="L7:M7"/>
-    <mergeCell ref="N7:O7"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="L4:M4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="J4:K4"/>
     <mergeCell ref="C21:C22"/>
     <mergeCell ref="L13:M13"/>
     <mergeCell ref="D17:E17"/>
@@ -3403,6 +3396,45 @@
     <mergeCell ref="F18:G18"/>
     <mergeCell ref="H15:I15"/>
     <mergeCell ref="J15:K15"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="N7:O7"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="N9:O9"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="L11:M11"/>
+    <mergeCell ref="N11:O11"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="N15:O15"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="N13:O13"/>
+    <mergeCell ref="L15:M15"/>
+    <mergeCell ref="N18:O18"/>
+    <mergeCell ref="N17:O17"/>
+    <mergeCell ref="L18:M18"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="L17:M17"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="J18:K18"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
@@ -3422,7 +3454,7 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -3465,10 +3497,10 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="101"/>
-      <c r="B4" s="188" t="s">
+      <c r="B4" s="182" t="s">
         <v>86</v>
       </c>
-      <c r="C4" s="189"/>
+      <c r="C4" s="183"/>
       <c r="D4" s="6">
         <v>600000</v>
       </c>
@@ -3480,10 +3512,10 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="101"/>
-      <c r="B5" s="184" t="s">
+      <c r="B5" s="180" t="s">
         <v>118</v>
       </c>
-      <c r="C5" s="185"/>
+      <c r="C5" s="181"/>
       <c r="D5" s="4">
         <f>IF('HW y SW'!C5=0,100000,0)</f>
         <v>0</v>
@@ -3496,10 +3528,10 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="101"/>
-      <c r="B6" s="184" t="s">
+      <c r="B6" s="180" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="185"/>
+      <c r="C6" s="181"/>
       <c r="D6" s="4">
         <f>PERSONAL!E12</f>
         <v>8000000</v>
@@ -3512,10 +3544,10 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="101"/>
-      <c r="B7" s="184" t="s">
+      <c r="B7" s="180" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="185"/>
+      <c r="C7" s="181"/>
       <c r="D7" s="4">
         <v>100000</v>
       </c>
@@ -3527,10 +3559,10 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="101"/>
-      <c r="B8" s="184" t="s">
+      <c r="B8" s="180" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="185"/>
+      <c r="C8" s="181"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4">
         <v>13000</v>
@@ -3539,10 +3571,10 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="101"/>
-      <c r="B9" s="184" t="s">
+      <c r="B9" s="180" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="185"/>
+      <c r="C9" s="181"/>
       <c r="D9" s="4">
         <v>50000</v>
       </c>
@@ -3554,10 +3586,10 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="101"/>
-      <c r="B10" s="184" t="s">
+      <c r="B10" s="180" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="185"/>
+      <c r="C10" s="181"/>
       <c r="D10" s="4">
         <v>45000</v>
       </c>
@@ -3569,10 +3601,10 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="101"/>
-      <c r="B11" s="184" t="s">
+      <c r="B11" s="180" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="185"/>
+      <c r="C11" s="181"/>
       <c r="D11" s="4">
         <v>45000</v>
       </c>
@@ -3584,10 +3616,10 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="101"/>
-      <c r="B12" s="184" t="s">
+      <c r="B12" s="180" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="185"/>
+      <c r="C12" s="181"/>
       <c r="D12" s="4">
         <f>'CREACIÓN CURSOS'!D9</f>
         <v>1100000</v>
@@ -3600,10 +3632,10 @@
     </row>
     <row r="13" spans="1:6" ht="13" thickBot="1">
       <c r="A13" s="101"/>
-      <c r="B13" s="180" t="s">
+      <c r="B13" s="184" t="s">
         <v>120</v>
       </c>
-      <c r="C13" s="182"/>
+      <c r="C13" s="186"/>
       <c r="D13" s="5">
         <f>SUM(D4:D12)*0.02</f>
         <v>198800</v>
@@ -3620,7 +3652,7 @@
       <c r="C14" s="154" t="s">
         <v>44</v>
       </c>
-      <c r="D14" s="183"/>
+      <c r="D14" s="187"/>
       <c r="E14" s="11">
         <f>SUM(E4:E13)</f>
         <v>113378600</v>
@@ -3645,10 +3677,10 @@
     </row>
     <row r="17" spans="1:8" ht="13" thickBot="1">
       <c r="A17" s="101"/>
-      <c r="B17" s="186" t="s">
+      <c r="B17" s="188" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="187"/>
+      <c r="C17" s="189"/>
       <c r="D17" s="30" t="s">
         <v>61</v>
       </c>
@@ -3673,10 +3705,10 @@
     </row>
     <row r="19" spans="1:8" ht="13" thickBot="1">
       <c r="A19" s="101"/>
-      <c r="B19" s="180" t="s">
+      <c r="B19" s="184" t="s">
         <v>43</v>
       </c>
-      <c r="C19" s="181"/>
+      <c r="C19" s="185"/>
       <c r="D19" s="100">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -3703,6 +3735,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B17:C17"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B4:C4"/>
@@ -3710,12 +3748,6 @@
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B17:C17"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
@@ -4187,7 +4219,7 @@
   <sheetData>
     <row r="1" spans="2:5" ht="13" thickBot="1"/>
     <row r="2" spans="2:5" ht="13" thickBot="1">
-      <c r="D2" s="186" t="s">
+      <c r="D2" s="188" t="s">
         <v>39</v>
       </c>
       <c r="E2" s="190"/>
@@ -4367,7 +4399,7 @@
       <c r="C4" s="191" t="s">
         <v>112</v>
       </c>
-      <c r="D4" s="183"/>
+      <c r="D4" s="187"/>
     </row>
     <row r="5" spans="3:10" ht="13" thickBot="1">
       <c r="C5" s="27" t="s">

</xml_diff>